<commit_message>
scenario updates from mtg 02_06_14
</commit_message>
<xml_diff>
--- a/docs/Project BackLog.xlsx
+++ b/docs/Project BackLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Add a panel to allow users to customize/filter what/how they see info</t>
   </si>
@@ -41,10 +41,31 @@
     <t>Collapse/expand on tree view</t>
   </si>
   <si>
-    <t>Project hours invested. So far the project is defined on;y in calendar time. There will also be time spent/invested in the project</t>
-  </si>
-  <si>
     <t>once the project hours feature is implemented, the user will need to be able to update the hours spent.</t>
+  </si>
+  <si>
+    <t>alternate project/task delete. in project properties panel</t>
+  </si>
+  <si>
+    <t>better tree navigation system: hand grab and drag, diagonal arrow, more intuitive</t>
+  </si>
+  <si>
+    <t>Project progress incorporated visually into tree/outline views</t>
+  </si>
+  <si>
+    <t>Project hours invested. So far the project is defined only in calendar time. There will also be time spent/invested in the project</t>
+  </si>
+  <si>
+    <t>when project/task is completed, fireworks, music, congratulations</t>
+  </si>
+  <si>
+    <t>project accomplishments share on facebook</t>
+  </si>
+  <si>
+    <t>project documentation - add pictures of project in progress and on completion</t>
+  </si>
+  <si>
+    <t>project archiving</t>
   </si>
 </sst>
 </file>
@@ -362,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,12 +421,47 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates from Monday meeting
</commit_message>
<xml_diff>
--- a/docs/Project BackLog.xlsx
+++ b/docs/Project BackLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Add a panel to allow users to customize/filter what/how they see info</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>project archiving</t>
+  </si>
+  <si>
+    <t>user shares projects in publicly available repository - devin says "project sharing privileges"</t>
   </si>
 </sst>
 </file>
@@ -383,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,6 +467,11 @@
         <v>13</v>
       </c>
     </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>